<commit_message>
Remove build e __pycache__ do rastreamento
</commit_message>
<xml_diff>
--- a/atestados.xlsx
+++ b/atestados.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://spsenacbr-my.sharepoint.com/personal/lucas_fbarros_sp_senac_br/Documents/Documentos/autoAtestado/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="484" documentId="11_AD4D361C20488DEA4E38A0581C9F55E45BDEDD97" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{99EED0AC-F017-40B0-B933-1D50A16EBE84}"/>
+  <xr:revisionPtr revIDLastSave="485" documentId="11_AD4D361C20488DEA4E38A0581C9F55E45BDEDD97" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B2693343-C9A4-4388-B482-DE4BC2933A0A}"/>
   <bookViews>
-    <workbookView xWindow="11100" yWindow="3315" windowWidth="14070" windowHeight="12150" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -393,7 +393,7 @@
   <dimension ref="A1:E362"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="B2:E8"/>
+      <selection activeCell="B2" sqref="B2:D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -423,15 +423,27 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B2" s="5"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
+      <c r="B2" s="5">
+        <v>1143120270</v>
+      </c>
+      <c r="C2" s="6">
+        <v>45897</v>
+      </c>
+      <c r="D2" s="6">
+        <v>45897</v>
+      </c>
       <c r="E2" s="3"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B3" s="7"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="6"/>
+      <c r="B3" s="7">
+        <v>1143140289</v>
+      </c>
+      <c r="C3" s="8">
+        <v>45898</v>
+      </c>
+      <c r="D3" s="6">
+        <v>45898</v>
+      </c>
       <c r="E3" s="3"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Atualiza AutoAtestado: configurações, UI, barra de progresso e status em tempo real
</commit_message>
<xml_diff>
--- a/atestados.xlsx
+++ b/atestados.xlsx
@@ -1,24 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://spsenacbr-my.sharepoint.com/personal/lucas_fbarros_sp_senac_br/Documents/Documentos/autoAtestado/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="488" documentId="11_AD4D361C20488DEA4E38A0581C9F55E45BDEDD97" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{45F05BA1-D544-48F7-8C06-156ABA630F65}"/>
+  <xr:revisionPtr revIDLastSave="490" documentId="11_AD4D361C20488DEA4E38A0581C9F55E45BDEDD97" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{41A2EEAA-676A-4020-B393-7CAC424C7A52}"/>
   <bookViews>
-    <workbookView xWindow="540" yWindow="1515" windowWidth="14070" windowHeight="12150" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1065" yWindow="1950" windowWidth="27735" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -390,7 +401,7 @@
   <dimension ref="A1:E361"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:D2"/>
+      <selection activeCell="B3" sqref="B3:D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -420,41 +431,77 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B2" s="5"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
+      <c r="B2" s="5">
+        <v>1142942811</v>
+      </c>
+      <c r="C2" s="6">
+        <v>45978</v>
+      </c>
+      <c r="D2" s="6">
+        <v>45978</v>
+      </c>
       <c r="E2" s="3"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B3" s="5"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="6"/>
+      <c r="B3" s="5">
+        <v>1143140284</v>
+      </c>
+      <c r="C3" s="7">
+        <v>45972</v>
+      </c>
+      <c r="D3" s="6">
+        <v>45972</v>
+      </c>
       <c r="E3" s="3"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
-      <c r="B4" s="5"/>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
+      <c r="B4" s="5">
+        <v>1142948325</v>
+      </c>
+      <c r="C4" s="6">
+        <v>45974</v>
+      </c>
+      <c r="D4" s="6">
+        <v>45974</v>
+      </c>
       <c r="E4" s="4"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
-      <c r="B5" s="5"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="6"/>
+      <c r="B5" s="5">
+        <v>1142932857</v>
+      </c>
+      <c r="C5" s="7">
+        <v>45973</v>
+      </c>
+      <c r="D5" s="6">
+        <v>45973</v>
+      </c>
       <c r="E5" s="4"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B6" s="5"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
+      <c r="B6" s="5">
+        <v>1142905695</v>
+      </c>
+      <c r="C6" s="6">
+        <v>45972</v>
+      </c>
+      <c r="D6" s="6">
+        <v>45973</v>
+      </c>
       <c r="E6" s="3"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B7" s="5"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
+      <c r="B7" s="5">
+        <v>1143164684</v>
+      </c>
+      <c r="C7" s="6">
+        <v>45978</v>
+      </c>
+      <c r="D7" s="6">
+        <v>45978</v>
+      </c>
       <c r="E7" s="3"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>